<commit_message>
edited my phone number
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\staffcard\CS335\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8B722D-3279-45AC-A3BB-BD0E9F041E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B74F6D-B8DE-4D28-B389-5F7EC9F703B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="15375" windowHeight="8325" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -3996,14 +3996,14 @@
       <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="9.8125" customWidth="1"/>
-    <col min="11" max="11" width="9.8125" customWidth="1"/>
+    <col min="5" max="5" width="9.875" customWidth="1"/>
+    <col min="11" max="11" width="9.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4041,7 +4041,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4079,7 +4079,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -4155,7 +4155,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -4269,7 +4269,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -4307,7 +4307,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -4345,7 +4345,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>82</v>
       </c>
@@ -4383,7 +4383,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>90</v>
       </c>
@@ -4421,7 +4421,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>98</v>
       </c>
@@ -4459,7 +4459,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>106</v>
       </c>
@@ -4497,7 +4497,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>113</v>
       </c>
@@ -4535,7 +4535,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>121</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>130</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>138</v>
       </c>
@@ -4649,7 +4649,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>146</v>
       </c>
@@ -4687,7 +4687,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>154</v>
       </c>
@@ -4725,7 +4725,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>163</v>
       </c>
@@ -4763,7 +4763,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>171</v>
       </c>
@@ -4801,7 +4801,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>179</v>
       </c>
@@ -4839,7 +4839,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>187</v>
       </c>
@@ -4877,7 +4877,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>195</v>
       </c>
@@ -4915,7 +4915,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>203</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>212</v>
       </c>
@@ -4991,7 +4991,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>221</v>
       </c>
@@ -5029,7 +5029,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>229</v>
       </c>
@@ -5067,7 +5067,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>237</v>
       </c>
@@ -5105,7 +5105,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>245</v>
       </c>
@@ -5143,7 +5143,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>253</v>
       </c>
@@ -5181,7 +5181,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>261</v>
       </c>
@@ -5219,7 +5219,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>269</v>
       </c>
@@ -5257,7 +5257,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>277</v>
       </c>
@@ -5295,7 +5295,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>286</v>
       </c>
@@ -5333,7 +5333,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>295</v>
       </c>
@@ -5371,7 +5371,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>303</v>
       </c>
@@ -5409,7 +5409,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>312</v>
       </c>
@@ -5447,7 +5447,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>320</v>
       </c>
@@ -5485,7 +5485,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>328</v>
       </c>
@@ -5523,7 +5523,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>337</v>
       </c>
@@ -5561,7 +5561,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>345</v>
       </c>
@@ -5599,7 +5599,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>353</v>
       </c>
@@ -5637,7 +5637,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>361</v>
       </c>
@@ -5675,7 +5675,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>369</v>
       </c>
@@ -5713,7 +5713,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>377</v>
       </c>
@@ -5751,7 +5751,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>385</v>
       </c>
@@ -5789,7 +5789,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>393</v>
       </c>
@@ -5827,7 +5827,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>401</v>
       </c>
@@ -5865,7 +5865,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>409</v>
       </c>
@@ -5903,7 +5903,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>417</v>
       </c>
@@ -5941,7 +5941,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>425</v>
       </c>
@@ -5979,7 +5979,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>433</v>
       </c>
@@ -6017,7 +6017,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>441</v>
       </c>
@@ -6055,7 +6055,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>449</v>
       </c>
@@ -6093,7 +6093,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>457</v>
       </c>
@@ -6131,7 +6131,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>465</v>
       </c>
@@ -6169,7 +6169,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>473</v>
       </c>
@@ -6207,7 +6207,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>482</v>
       </c>
@@ -6245,7 +6245,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>489</v>
       </c>
@@ -6283,7 +6283,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>497</v>
       </c>
@@ -6321,7 +6321,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>506</v>
       </c>
@@ -6359,7 +6359,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>514</v>
       </c>
@@ -6397,7 +6397,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>522</v>
       </c>
@@ -6435,7 +6435,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>531</v>
       </c>
@@ -6473,7 +6473,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>539</v>
       </c>
@@ -6511,7 +6511,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>547</v>
       </c>
@@ -6549,7 +6549,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>555</v>
       </c>
@@ -6587,7 +6587,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>563</v>
       </c>
@@ -6625,7 +6625,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>572</v>
       </c>
@@ -6663,7 +6663,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>580</v>
       </c>
@@ -6701,7 +6701,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>588</v>
       </c>
@@ -6739,7 +6739,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>596</v>
       </c>
@@ -6777,7 +6777,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>604</v>
       </c>
@@ -6815,7 +6815,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>612</v>
       </c>
@@ -6853,7 +6853,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>620</v>
       </c>
@@ -6891,7 +6891,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>629</v>
       </c>
@@ -6929,7 +6929,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>636</v>
       </c>
@@ -6967,7 +6967,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>643</v>
       </c>
@@ -7005,7 +7005,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>651</v>
       </c>
@@ -7043,7 +7043,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>659</v>
       </c>
@@ -7081,7 +7081,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>667</v>
       </c>
@@ -7119,7 +7119,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>675</v>
       </c>
@@ -7157,7 +7157,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>684</v>
       </c>
@@ -7195,7 +7195,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>691</v>
       </c>
@@ -7233,7 +7233,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>699</v>
       </c>
@@ -7271,7 +7271,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>707</v>
       </c>
@@ -7309,7 +7309,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>715</v>
       </c>
@@ -7347,7 +7347,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>723</v>
       </c>
@@ -7385,7 +7385,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>731</v>
       </c>
@@ -7423,7 +7423,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>739</v>
       </c>
@@ -7461,7 +7461,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>747</v>
       </c>
@@ -7499,7 +7499,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>755</v>
       </c>
@@ -7537,7 +7537,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>763</v>
       </c>
@@ -7575,7 +7575,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>771</v>
       </c>
@@ -7613,7 +7613,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>773</v>
       </c>
@@ -7651,7 +7651,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>781</v>
       </c>
@@ -7689,7 +7689,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>789</v>
       </c>
@@ -7727,7 +7727,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>797</v>
       </c>
@@ -7765,7 +7765,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>805</v>
       </c>
@@ -7803,7 +7803,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>813</v>
       </c>
@@ -7841,7 +7841,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>821</v>
       </c>
@@ -7879,7 +7879,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>829</v>
       </c>
@@ -7914,7 +7914,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>836</v>
       </c>
@@ -7954,7 +7954,7 @@
       <c r="M104" s="8"/>
       <c r="P104" s="1"/>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>843</v>
       </c>
@@ -7992,7 +7992,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>851</v>
       </c>
@@ -8030,7 +8030,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>44518.9544328704</v>
       </c>
@@ -8068,7 +8068,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>866</v>
       </c>
@@ -8106,7 +8106,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>874</v>
       </c>
@@ -8144,7 +8144,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>883</v>
       </c>
@@ -8182,7 +8182,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>891</v>
       </c>
@@ -8220,7 +8220,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>893</v>
       </c>
@@ -8258,7 +8258,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>901</v>
       </c>
@@ -8293,7 +8293,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>903</v>
       </c>
@@ -8331,7 +8331,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>911</v>
       </c>
@@ -8369,7 +8369,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>919</v>
       </c>
@@ -8407,7 +8407,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>927</v>
       </c>
@@ -8445,7 +8445,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>934</v>
       </c>
@@ -8483,7 +8483,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>942</v>
       </c>
@@ -8521,7 +8521,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>950</v>
       </c>
@@ -8559,7 +8559,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>957</v>
       </c>
@@ -8597,7 +8597,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>965</v>
       </c>
@@ -8635,7 +8635,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>973</v>
       </c>
@@ -8670,7 +8670,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>483</v>
       </c>
@@ -8705,7 +8705,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>977</v>
       </c>
@@ -8731,7 +8731,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>523</v>
       </c>
@@ -8754,7 +8754,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>982</v>
       </c>
@@ -8810,16 +8810,16 @@
       <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="15.8125" customWidth="1"/>
-    <col min="5" max="5" width="14.5625" customWidth="1"/>
-    <col min="6" max="6" width="9.8125" customWidth="1"/>
+    <col min="4" max="4" width="15.875" customWidth="1"/>
+    <col min="5" max="5" width="14.625" customWidth="1"/>
+    <col min="6" max="6" width="9.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>990</v>
       </c>
@@ -8851,7 +8851,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>997</v>
       </c>
@@ -8883,7 +8883,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1000</v>
       </c>
@@ -8915,7 +8915,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -8947,7 +8947,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1001</v>
       </c>
@@ -8979,7 +8979,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1003</v>
       </c>
@@ -9011,7 +9011,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1004</v>
       </c>
@@ -9043,7 +9043,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1006</v>
       </c>
@@ -9075,7 +9075,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1007</v>
       </c>
@@ -9107,7 +9107,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1008</v>
       </c>
@@ -9139,7 +9139,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1009</v>
       </c>
@@ -9171,7 +9171,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1010</v>
       </c>
@@ -9203,7 +9203,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1011</v>
       </c>
@@ -9235,7 +9235,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1012</v>
       </c>
@@ -9267,7 +9267,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1013</v>
       </c>
@@ -9299,7 +9299,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1014</v>
       </c>
@@ -9331,7 +9331,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1015</v>
       </c>
@@ -9363,7 +9363,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>1016</v>
       </c>
@@ -9395,7 +9395,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1017</v>
       </c>
@@ -9427,7 +9427,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1018</v>
       </c>
@@ -9459,7 +9459,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1019</v>
       </c>
@@ -9491,7 +9491,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>1020</v>
       </c>
@@ -9523,7 +9523,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1021</v>
       </c>
@@ -9555,7 +9555,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1023</v>
       </c>
@@ -9587,7 +9587,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>1024</v>
       </c>
@@ -9619,7 +9619,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>1025</v>
       </c>
@@ -9651,7 +9651,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1026</v>
       </c>
@@ -9683,7 +9683,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1027</v>
       </c>
@@ -9715,7 +9715,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1028</v>
       </c>
@@ -9747,7 +9747,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1029</v>
       </c>
@@ -9779,7 +9779,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1030</v>
       </c>
@@ -9811,7 +9811,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1031</v>
       </c>
@@ -9843,7 +9843,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1033</v>
       </c>
@@ -9875,7 +9875,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1034</v>
       </c>
@@ -9907,7 +9907,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1035</v>
       </c>
@@ -9939,7 +9939,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1037</v>
       </c>
@@ -9971,7 +9971,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1038</v>
       </c>
@@ -10003,7 +10003,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>1039</v>
       </c>
@@ -10035,7 +10035,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>1040</v>
       </c>
@@ -10067,7 +10067,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>1041</v>
       </c>
@@ -10099,7 +10099,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>1042</v>
       </c>
@@ -10131,7 +10131,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>1043</v>
       </c>
@@ -10163,7 +10163,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>1044</v>
       </c>
@@ -10195,7 +10195,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>1045</v>
       </c>
@@ -10227,7 +10227,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>1046</v>
       </c>
@@ -10259,7 +10259,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>1047</v>
       </c>
@@ -10291,7 +10291,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>1048</v>
       </c>
@@ -10323,7 +10323,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>1049</v>
       </c>
@@ -10355,7 +10355,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>1050</v>
       </c>
@@ -10387,7 +10387,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>1051</v>
       </c>
@@ -10419,7 +10419,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>1053</v>
       </c>
@@ -10451,7 +10451,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>1054</v>
       </c>
@@ -10483,7 +10483,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>1055</v>
       </c>
@@ -10515,7 +10515,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>1056</v>
       </c>
@@ -10547,7 +10547,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>1057</v>
       </c>
@@ -10579,7 +10579,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>1058</v>
       </c>
@@ -10611,7 +10611,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>1059</v>
       </c>
@@ -10643,7 +10643,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>1061</v>
       </c>
@@ -10675,7 +10675,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>1062</v>
       </c>
@@ -10707,7 +10707,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>1063</v>
       </c>
@@ -10739,7 +10739,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>1064</v>
       </c>
@@ -10771,7 +10771,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>1065</v>
       </c>
@@ -10803,7 +10803,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>1066</v>
       </c>
@@ -10835,7 +10835,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>1067</v>
       </c>
@@ -10867,7 +10867,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>1068</v>
       </c>
@@ -10899,7 +10899,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>1069</v>
       </c>
@@ -10931,7 +10931,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>1070</v>
       </c>
@@ -10963,7 +10963,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>1071</v>
       </c>
@@ -10995,7 +10995,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>1072</v>
       </c>
@@ -11027,7 +11027,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>1073</v>
       </c>
@@ -11059,7 +11059,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>1074</v>
       </c>
@@ -11091,7 +11091,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>1075</v>
       </c>
@@ -11123,7 +11123,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>1076</v>
       </c>
@@ -11155,7 +11155,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>1077</v>
       </c>
@@ -11187,7 +11187,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>1078</v>
       </c>
@@ -11219,7 +11219,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>1079</v>
       </c>
@@ -11251,7 +11251,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>1080</v>
       </c>
@@ -11283,7 +11283,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>1082</v>
       </c>
@@ -11315,7 +11315,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>1083</v>
       </c>
@@ -11347,7 +11347,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>1084</v>
       </c>
@@ -11379,7 +11379,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>1085</v>
       </c>
@@ -11411,7 +11411,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>1086</v>
       </c>
@@ -11443,7 +11443,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>1087</v>
       </c>
@@ -11475,7 +11475,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>1088</v>
       </c>
@@ -11507,7 +11507,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>1089</v>
       </c>
@@ -11539,7 +11539,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>1090</v>
       </c>
@@ -11571,7 +11571,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>1091</v>
       </c>
@@ -11603,7 +11603,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>1092</v>
       </c>
@@ -11635,7 +11635,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>1093</v>
       </c>
@@ -11667,7 +11667,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>1094</v>
       </c>
@@ -11699,7 +11699,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>1095</v>
       </c>
@@ -11731,7 +11731,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>1096</v>
       </c>
@@ -11763,7 +11763,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>1097</v>
       </c>
@@ -11795,7 +11795,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>1098</v>
       </c>
@@ -11827,7 +11827,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>1099</v>
       </c>
@@ -11859,7 +11859,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>1100</v>
       </c>
@@ -11891,7 +11891,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>1101</v>
       </c>
@@ -11923,7 +11923,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>1102</v>
       </c>
@@ -11955,7 +11955,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>1103</v>
       </c>
@@ -11987,7 +11987,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>1104</v>
       </c>
@@ -12019,7 +12019,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>1106</v>
       </c>
@@ -12051,7 +12051,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>1107</v>
       </c>
@@ -12080,7 +12080,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>1108</v>
       </c>
@@ -12109,7 +12109,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>1112</v>
       </c>
@@ -12141,7 +12141,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>1114</v>
       </c>
@@ -12173,7 +12173,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>1115</v>
       </c>
@@ -12205,7 +12205,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>1117</v>
       </c>
@@ -12237,7 +12237,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>1118</v>
       </c>
@@ -12269,7 +12269,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>1119</v>
       </c>
@@ -12301,7 +12301,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>1120</v>
       </c>
@@ -12333,7 +12333,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>1121</v>
       </c>
@@ -12362,7 +12362,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>1122</v>
       </c>
@@ -12394,7 +12394,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>1125</v>
       </c>
@@ -12426,7 +12426,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>1133</v>
       </c>
@@ -12458,7 +12458,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>1134</v>
       </c>
@@ -12490,7 +12490,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>117</v>
       </c>
@@ -12535,22 +12535,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K119" sqref="K119"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="16.5" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="9.8125" customWidth="1"/>
-    <col min="7" max="7" width="29.1875" style="5" customWidth="1"/>
-    <col min="9" max="9" width="17.0625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="30.1875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="9.875" customWidth="1"/>
+    <col min="7" max="7" width="29.25" style="5" customWidth="1"/>
+    <col min="9" max="9" width="17.125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="30.25" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>990</v>
       </c>
@@ -12582,7 +12582,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>997</v>
       </c>
@@ -12614,7 +12614,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1000</v>
       </c>
@@ -12646,7 +12646,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -12678,7 +12678,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1001</v>
       </c>
@@ -12710,7 +12710,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1003</v>
       </c>
@@ -12742,7 +12742,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1004</v>
       </c>
@@ -12774,7 +12774,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1006</v>
       </c>
@@ -12806,7 +12806,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1007</v>
       </c>
@@ -12838,7 +12838,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1008</v>
       </c>
@@ -12870,7 +12870,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1009</v>
       </c>
@@ -12902,7 +12902,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1010</v>
       </c>
@@ -12934,7 +12934,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1011</v>
       </c>
@@ -12966,7 +12966,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1012</v>
       </c>
@@ -12998,7 +12998,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1013</v>
       </c>
@@ -13030,7 +13030,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1014</v>
       </c>
@@ -13062,7 +13062,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1015</v>
       </c>
@@ -13094,7 +13094,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>1016</v>
       </c>
@@ -13126,7 +13126,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1017</v>
       </c>
@@ -13158,7 +13158,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1018</v>
       </c>
@@ -13190,7 +13190,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1019</v>
       </c>
@@ -13222,7 +13222,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>1020</v>
       </c>
@@ -13254,7 +13254,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1021</v>
       </c>
@@ -13286,7 +13286,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1023</v>
       </c>
@@ -13318,7 +13318,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>1024</v>
       </c>
@@ -13350,7 +13350,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>1025</v>
       </c>
@@ -13382,7 +13382,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1026</v>
       </c>
@@ -13414,7 +13414,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1027</v>
       </c>
@@ -13446,7 +13446,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1028</v>
       </c>
@@ -13478,7 +13478,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1029</v>
       </c>
@@ -13510,7 +13510,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1030</v>
       </c>
@@ -13542,7 +13542,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1031</v>
       </c>
@@ -13574,7 +13574,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1033</v>
       </c>
@@ -13606,7 +13606,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1034</v>
       </c>
@@ -13638,7 +13638,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1035</v>
       </c>
@@ -13670,7 +13670,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1037</v>
       </c>
@@ -13702,7 +13702,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1038</v>
       </c>
@@ -13734,7 +13734,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>1039</v>
       </c>
@@ -13766,7 +13766,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>1040</v>
       </c>
@@ -13798,7 +13798,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>1041</v>
       </c>
@@ -13830,7 +13830,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>1042</v>
       </c>
@@ -13862,7 +13862,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>1043</v>
       </c>
@@ -13894,7 +13894,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>1044</v>
       </c>
@@ -13926,7 +13926,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>1045</v>
       </c>
@@ -13958,7 +13958,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>1046</v>
       </c>
@@ -13990,7 +13990,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>1047</v>
       </c>
@@ -14022,7 +14022,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>1048</v>
       </c>
@@ -14054,7 +14054,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>1049</v>
       </c>
@@ -14086,7 +14086,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>1050</v>
       </c>
@@ -14118,7 +14118,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>1051</v>
       </c>
@@ -14150,7 +14150,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>1053</v>
       </c>
@@ -14182,7 +14182,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>1054</v>
       </c>
@@ -14214,7 +14214,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>1055</v>
       </c>
@@ -14246,7 +14246,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>1056</v>
       </c>
@@ -14278,7 +14278,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>1057</v>
       </c>
@@ -14310,7 +14310,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>1058</v>
       </c>
@@ -14342,7 +14342,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>1059</v>
       </c>
@@ -14374,7 +14374,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>1061</v>
       </c>
@@ -14406,7 +14406,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>1062</v>
       </c>
@@ -14438,7 +14438,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>1063</v>
       </c>
@@ -14470,7 +14470,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>1064</v>
       </c>
@@ -14502,7 +14502,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>1065</v>
       </c>
@@ -14534,7 +14534,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>1066</v>
       </c>
@@ -14566,7 +14566,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>1067</v>
       </c>
@@ -14598,7 +14598,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>1068</v>
       </c>
@@ -14630,7 +14630,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>1069</v>
       </c>
@@ -14662,7 +14662,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>1070</v>
       </c>
@@ -14694,7 +14694,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>1071</v>
       </c>
@@ -14726,7 +14726,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>1072</v>
       </c>
@@ -14758,7 +14758,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>1073</v>
       </c>
@@ -14790,7 +14790,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>1074</v>
       </c>
@@ -14822,7 +14822,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>1075</v>
       </c>
@@ -14854,7 +14854,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>1076</v>
       </c>
@@ -14886,7 +14886,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>1077</v>
       </c>
@@ -14918,7 +14918,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>1078</v>
       </c>
@@ -14950,7 +14950,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>1079</v>
       </c>
@@ -14982,7 +14982,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>1080</v>
       </c>
@@ -15014,7 +15014,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>1082</v>
       </c>
@@ -15046,7 +15046,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>1083</v>
       </c>
@@ -15078,7 +15078,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>1084</v>
       </c>
@@ -15110,7 +15110,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>1085</v>
       </c>
@@ -15142,7 +15142,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>1086</v>
       </c>
@@ -15174,7 +15174,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>1087</v>
       </c>
@@ -15206,7 +15206,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>1088</v>
       </c>
@@ -15238,7 +15238,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>1089</v>
       </c>
@@ -15270,7 +15270,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>1090</v>
       </c>
@@ -15302,7 +15302,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>1091</v>
       </c>
@@ -15334,7 +15334,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>1092</v>
       </c>
@@ -15363,7 +15363,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>1093</v>
       </c>
@@ -15392,7 +15392,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>1094</v>
       </c>
@@ -15424,7 +15424,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>1095</v>
       </c>
@@ -15456,7 +15456,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>1096</v>
       </c>
@@ -15488,7 +15488,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>1097</v>
       </c>
@@ -15520,7 +15520,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>1098</v>
       </c>
@@ -15537,7 +15537,7 @@
         <v>878</v>
       </c>
       <c r="F94" t="s">
-        <v>879</v>
+        <v>998</v>
       </c>
       <c r="G94" s="5" t="s">
         <v>880</v>
@@ -15552,7 +15552,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>1099</v>
       </c>
@@ -15584,7 +15584,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>1100</v>
       </c>
@@ -15616,7 +15616,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>1101</v>
       </c>
@@ -15648,7 +15648,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>1102</v>
       </c>
@@ -15677,7 +15677,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>1103</v>
       </c>
@@ -15709,7 +15709,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>1104</v>
       </c>
@@ -15741,7 +15741,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>1106</v>
       </c>
@@ -15773,7 +15773,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>1107</v>
       </c>
@@ -15805,7 +15805,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>1108</v>
       </c>
@@ -15837,7 +15837,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>1112</v>
       </c>
@@ -15869,7 +15869,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>1114</v>
       </c>
@@ -15901,7 +15901,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>1115</v>
       </c>
@@ -15933,7 +15933,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>1117</v>
       </c>
@@ -15965,7 +15965,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>1118</v>
       </c>
@@ -15997,7 +15997,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>1119</v>
       </c>
@@ -16029,7 +16029,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>1150</v>
       </c>
@@ -16061,7 +16061,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>1120</v>
       </c>
@@ -16093,7 +16093,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>1121</v>
       </c>
@@ -16125,7 +16125,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -16157,7 +16157,7 @@
         <v>1147</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -16189,7 +16189,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -16221,7 +16221,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -16250,7 +16250,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -16282,7 +16282,7 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>

</xml_diff>